<commit_message>
7rmart project second commit
</commit_message>
<xml_diff>
--- a/7rmart/src/test/resources/TestData.xlsx
+++ b/7rmart/src/test/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\eclipse-workspace\7Rmart\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\git\7rmartProject\7rmart\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C259C-B9BD-43BC-A9AC-141B669A6503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A63FF0-214A-466B-924C-5E9589974515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="5" xr2:uid="{DCEB16BB-26EA-4510-96A0-ADAFEB6CBD2A}"/>
+    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{DCEB16BB-26EA-4510-96A0-ADAFEB6CBD2A}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Arun(ho),Kottarakkara(po),Kollam</t>
+  </si>
+  <si>
+    <t>adminn123</t>
   </si>
 </sst>
 </file>
@@ -484,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1450D9-9E95-4DFD-9890-FF23014C5A3E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +530,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAFB7C8-0333-4E08-8DC6-926949DF70C4}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
7rmart project sixth commit
</commit_message>
<xml_diff>
--- a/7rmart/src/test/resources/TestData.xlsx
+++ b/7rmart/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\git\7rmartProject\7rmart\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A63FF0-214A-466B-924C-5E9589974515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEF5114-8B57-4C5B-9984-161D4EB8E7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{DCEB16BB-26EA-4510-96A0-ADAFEB6CBD2A}"/>
+    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="4" xr2:uid="{DCEB16BB-26EA-4510-96A0-ADAFEB6CBD2A}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpage" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>adminn123</t>
+  </si>
+  <si>
+    <t>Perfumes</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1450D9-9E95-4DFD-9890-FF23014C5A3E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -690,10 +693,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAD133F-A249-420D-9613-6137A8C221B9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,6 +736,17 @@
       </c>
       <c r="C3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>